<commit_message>
Use exogenous Carbon Intensity Ratios so LCFS works as a biofuel share requirement (PEI != 0 for biodiesel in BAU)
</commit_message>
<xml_diff>
--- a/InputData/trans/CIRbTF/Carbon Intensity Ratios by Transport Fuel.xlsx
+++ b/InputData/trans/CIRbTF/Carbon Intensity Ratios by Transport Fuel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\CIRbTF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\CIRbTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296B2019-D715-448B-9BDB-BB831A45902B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27420" windowHeight="11880"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,19 +429,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -448,57 +451,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -510,28 +513,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -539,7 +542,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -547,7 +550,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -555,7 +558,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -563,7 +566,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -571,15 +574,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -587,7 +590,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -595,7 +598,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -603,7 +606,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>

</xml_diff>